<commit_message>
docs: add document with some test cases
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/87c8305e0388e18c/Documents/Work/Hunty/Technical Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED7C3726-AEAC-4FCA-8F49-95FA4AFD1482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{ED7C3726-AEAC-4FCA-8F49-95FA4AFD1482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BBF798C-F19F-45B0-A1F9-606361DA3A30}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3436706F-8727-467D-B3C7-A1E57BCCE242}"/>
   </bookViews>
@@ -190,9 +190,6 @@
     <t>El usuario debe ser redirigido a una página que le confirma su correcto registro en la plataforma y debe estar con su sesion iniciada</t>
   </si>
   <si>
-    <t xml:space="preserve">El usuario debe estar en la inicio de sesion y tener un cuenta registrada	</t>
-  </si>
-  <si>
     <t>1. Dar click en el botón de "Recuperar Contraseña" 
 2. Introducir el email de la cuenta 
 3. Hacer clic en el botón de recuperación de contraseña</t>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>TEST CASES `http://opencart.abstracta.us/`</t>
+  </si>
+  <si>
+    <t>El usuario debe estar en la inicio de sesion y tener un cuenta registrada</t>
   </si>
 </sst>
 </file>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363B97F7-6502-44F7-883E-A16A5A81A93C}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -659,7 +659,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -774,13 +774,13 @@
         <v>17</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>32</v>
@@ -803,7 +803,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>34</v>
@@ -820,7 +820,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>16</v>
@@ -835,13 +835,13 @@
         <v>33</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="85.5" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>27</v>
@@ -925,7 +925,7 @@
         <v>36</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>37</v>
@@ -936,7 +936,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>16</v>
@@ -948,16 +948,16 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
@@ -983,7 +983,7 @@
         <v>40</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>39</v>

</xml_diff>